<commit_message>
Selenium Grid 4 working as expected using docker-compose.yml
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -565,7 +565,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>5.048061116E9</v>
+        <v>9.601352233E9</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
@@ -594,7 +594,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>2.5315361E7</v>
+        <v>7.667286552E9</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>

</xml_diff>